<commit_message>
half done with deleting and reordering
</commit_message>
<xml_diff>
--- a/feature_testing/full_feature_summary.xlsx
+++ b/feature_testing/full_feature_summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="22940" yWindow="0" windowWidth="15460" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="70">
   <si>
     <t>age</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>variable</t>
+  </si>
+  <si>
+    <t>deleted</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -291,8 +297,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -359,7 +369,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -388,6 +398,8 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -416,6 +428,8 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -747,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="AP4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -5776,15 +5790,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D2:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -5792,517 +5809,712 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>6.7134453251630449E-2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>4.9269499483078259E-2</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>4.3366350143000006E-2</v>
       </c>
       <c r="B4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4.1627834156331818E-2</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>4.017628903265455E-2</v>
       </c>
       <c r="B6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>3.9317547189813631E-2</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>3.7446796103504543E-2</v>
       </c>
       <c r="B8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>3.7038871262581811E-2</v>
       </c>
       <c r="B9" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>3.6844189148622732E-2</v>
       </c>
       <c r="B10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>3.6674883790568179E-2</v>
       </c>
       <c r="B11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>3.428109684026364E-2</v>
       </c>
       <c r="B12" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>3.3037224266140912E-2</v>
       </c>
       <c r="B13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>3.2183234398740906E-2</v>
       </c>
       <c r="B14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>3.0577132746727274E-2</v>
       </c>
       <c r="B15" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>3.0117097758390911E-2</v>
       </c>
       <c r="B16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>2.9806466931509092E-2</v>
       </c>
       <c r="B17" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>2.9214750794495446E-2</v>
       </c>
       <c r="B18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>2.6221428122690908E-2</v>
       </c>
       <c r="B19" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>2.3506248441495455E-2</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>2.1549565318059093E-2</v>
       </c>
       <c r="B21" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>2.067548943467273E-2</v>
       </c>
       <c r="B22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>1.998293870917273E-2</v>
       </c>
       <c r="B23" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>1.5971362453018181E-2</v>
       </c>
       <c r="B24" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>1.5210514870365219E-2</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>1.4471895346350001E-2</v>
       </c>
       <c r="B26" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>1.4081558636186086E-2</v>
       </c>
       <c r="B27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>1.3796385435289129E-2</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>1.3200372770273914E-2</v>
       </c>
       <c r="B29" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>1.305073489265182E-2</v>
       </c>
       <c r="B30" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>1.1773700008495216E-2</v>
       </c>
       <c r="B31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>1.1374816964996088E-2</v>
       </c>
       <c r="B32" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>1.0756037779543478E-2</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>9.9770015564339138E-3</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>9.4779892885130442E-3</v>
       </c>
       <c r="B35" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>9.1605724371547851E-3</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>8.6872520565469558E-3</v>
       </c>
       <c r="B37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>8.1390700069247871E-3</v>
       </c>
       <c r="B38" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>8.0390225510726127E-3</v>
       </c>
       <c r="B39" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>7.9850424811626092E-3</v>
       </c>
       <c r="B40" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>7.4462714566252168E-3</v>
       </c>
       <c r="B41" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>7.3916345701017395E-3</v>
       </c>
       <c r="B42" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>6.5180856439517381E-3</v>
       </c>
       <c r="B43" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>6.2798314241169564E-3</v>
       </c>
       <c r="B44" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>6.1041610451317398E-3</v>
       </c>
       <c r="B45" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>5.7652194370082606E-3</v>
       </c>
       <c r="B46" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>5.4247569727569576E-3</v>
       </c>
       <c r="B47" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>5.2816729149608695E-3</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>5.1528236184095657E-3</v>
       </c>
       <c r="B49" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>4.1163755219821739E-3</v>
       </c>
       <c r="B50" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>3.8062080407660877E-3</v>
       </c>
       <c r="B51" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>3.2939142339939139E-3</v>
       </c>
       <c r="B52" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>2.4032604290486958E-3</v>
       </c>
       <c r="B53" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>1.090099412876174E-3</v>
       </c>
       <c r="B54" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>8.9058068344500011E-4</v>
       </c>
       <c r="B55" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>7.7957421183265222E-4</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>7.2099957767608703E-4</v>
       </c>
       <c r="B57" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>4.8287647005413041E-4</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>4.4680197807000008E-4</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>4.2926325744621733E-4</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>3.8774555202691305E-4</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>3.1291200552990871E-4</v>
       </c>
       <c r="B62" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>5.4326336001418164E-5</v>
       </c>
       <c r="B63" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>4.7967975440741306E-5</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>4.5548340350777819E-5</v>
       </c>
       <c r="B65" t="s">
         <v>13</v>
       </c>
+      <c r="C65" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3">
+      <c r="C1048576" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:B65">
@@ -6311,6 +6523,7 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Space for people to enter their guesses. Need to compare that to the truth and assign them points.
</commit_message>
<xml_diff>
--- a/feature_testing/full_feature_summary.xlsx
+++ b/feature_testing/full_feature_summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="22940" yWindow="0" windowWidth="15460" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4400" yWindow="0" windowWidth="34000" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$BN$26</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$B$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$65</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -762,10 +762,10 @@
   <dimension ref="A1:BN26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AP4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AP24" sqref="AP24"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5790,10 +5790,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D2:D30"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.75"/>
@@ -5864,7 +5865,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" hidden="1">
       <c r="A7">
         <v>3.9317547189813631E-2</v>
       </c>
@@ -5875,7 +5876,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" hidden="1">
       <c r="A8">
         <v>3.7446796103504543E-2</v>
       </c>
@@ -5897,7 +5898,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" hidden="1">
       <c r="A10">
         <v>3.6844189148622732E-2</v>
       </c>
@@ -5908,7 +5909,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" hidden="1">
       <c r="A11">
         <v>3.6674883790568179E-2</v>
       </c>
@@ -5919,7 +5920,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" hidden="1">
       <c r="A12">
         <v>3.428109684026364E-2</v>
       </c>
@@ -6062,7 +6063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" hidden="1">
       <c r="A25">
         <v>1.5210514870365219E-2</v>
       </c>
@@ -6084,7 +6085,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" hidden="1">
       <c r="A27">
         <v>1.4081558636186086E-2</v>
       </c>
@@ -6095,7 +6096,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" hidden="1">
       <c r="A28">
         <v>1.3796385435289129E-2</v>
       </c>
@@ -6106,7 +6107,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" hidden="1">
       <c r="A29">
         <v>1.3200372770273914E-2</v>
       </c>
@@ -6128,7 +6129,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" hidden="1">
       <c r="A31">
         <v>1.1773700008495216E-2</v>
       </c>
@@ -6139,7 +6140,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" hidden="1">
       <c r="A32">
         <v>1.1374816964996088E-2</v>
       </c>
@@ -6150,7 +6151,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" hidden="1">
       <c r="A33">
         <v>1.0756037779543478E-2</v>
       </c>
@@ -6161,7 +6162,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" hidden="1">
       <c r="A34">
         <v>9.9770015564339138E-3</v>
       </c>
@@ -6172,7 +6173,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" hidden="1">
       <c r="A35">
         <v>9.4779892885130442E-3</v>
       </c>
@@ -6183,7 +6184,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" hidden="1">
       <c r="A36">
         <v>9.1605724371547851E-3</v>
       </c>
@@ -6194,7 +6195,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" hidden="1">
       <c r="A37">
         <v>8.6872520565469558E-3</v>
       </c>
@@ -6205,7 +6206,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" hidden="1">
       <c r="A38">
         <v>8.1390700069247871E-3</v>
       </c>
@@ -6216,7 +6217,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" hidden="1">
       <c r="A39">
         <v>8.0390225510726127E-3</v>
       </c>
@@ -6227,7 +6228,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" hidden="1">
       <c r="A40">
         <v>7.9850424811626092E-3</v>
       </c>
@@ -6238,7 +6239,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" hidden="1">
       <c r="A41">
         <v>7.4462714566252168E-3</v>
       </c>
@@ -6249,7 +6250,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" hidden="1">
       <c r="A42">
         <v>7.3916345701017395E-3</v>
       </c>
@@ -6260,7 +6261,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" hidden="1">
       <c r="A43">
         <v>6.5180856439517381E-3</v>
       </c>
@@ -6271,7 +6272,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" hidden="1">
       <c r="A44">
         <v>6.2798314241169564E-3</v>
       </c>
@@ -6282,7 +6283,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" hidden="1">
       <c r="A45">
         <v>6.1041610451317398E-3</v>
       </c>
@@ -6293,7 +6294,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" hidden="1">
       <c r="A46">
         <v>5.7652194370082606E-3</v>
       </c>
@@ -6304,7 +6305,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" hidden="1">
       <c r="A47">
         <v>5.4247569727569576E-3</v>
       </c>
@@ -6315,7 +6316,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" hidden="1">
       <c r="A48">
         <v>5.2816729149608695E-3</v>
       </c>
@@ -6326,7 +6327,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" hidden="1">
       <c r="A49">
         <v>5.1528236184095657E-3</v>
       </c>
@@ -6337,7 +6338,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" hidden="1">
       <c r="A50">
         <v>4.1163755219821739E-3</v>
       </c>
@@ -6348,7 +6349,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" hidden="1">
       <c r="A51">
         <v>3.8062080407660877E-3</v>
       </c>
@@ -6359,7 +6360,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" hidden="1">
       <c r="A52">
         <v>3.2939142339939139E-3</v>
       </c>
@@ -6370,7 +6371,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" hidden="1">
       <c r="A53">
         <v>2.4032604290486958E-3</v>
       </c>
@@ -6381,7 +6382,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" hidden="1">
       <c r="A54">
         <v>1.090099412876174E-3</v>
       </c>
@@ -6392,7 +6393,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" hidden="1">
       <c r="A55">
         <v>8.9058068344500011E-4</v>
       </c>
@@ -6403,7 +6404,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" hidden="1">
       <c r="A56">
         <v>7.7957421183265222E-4</v>
       </c>
@@ -6414,7 +6415,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" hidden="1">
       <c r="A57">
         <v>7.2099957767608703E-4</v>
       </c>
@@ -6425,7 +6426,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" hidden="1">
       <c r="A58">
         <v>4.8287647005413041E-4</v>
       </c>
@@ -6436,7 +6437,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" hidden="1">
       <c r="A59">
         <v>4.4680197807000008E-4</v>
       </c>
@@ -6447,7 +6448,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" hidden="1">
       <c r="A60">
         <v>4.2926325744621733E-4</v>
       </c>
@@ -6458,7 +6459,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" hidden="1">
       <c r="A61">
         <v>3.8774555202691305E-4</v>
       </c>
@@ -6469,7 +6470,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" hidden="1">
       <c r="A62">
         <v>3.1291200552990871E-4</v>
       </c>
@@ -6480,7 +6481,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" hidden="1">
       <c r="A63">
         <v>5.4326336001418164E-5</v>
       </c>
@@ -6491,7 +6492,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" hidden="1">
       <c r="A64">
         <v>4.7967975440741306E-5</v>
       </c>
@@ -6502,7 +6503,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" hidden="1">
       <c r="A65">
         <v>4.5548340350777819E-5</v>
       </c>
@@ -6517,10 +6518,10 @@
       <c r="C1048576" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B65">
-    <sortState ref="A2:B65">
-      <sortCondition descending="1" ref="A1:A65"/>
-    </sortState>
+  <autoFilter ref="A1:D65">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>